<commit_message>
Force update lote datacube
</commit_message>
<xml_diff>
--- a/data/metadata/Informe-05-050006-A-TC-TP.xlsx
+++ b/data/metadata/Informe-05-050006-A-TC-TP.xlsx
@@ -272,7 +272,7 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -385,7 +385,7 @@
         <v>30</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>26</v>
@@ -423,7 +423,7 @@
         <v>33</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>33</v>
@@ -461,7 +461,7 @@
         <v>39</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>40</v>

</xml_diff>